<commit_message>
Readding the timber types file
</commit_message>
<xml_diff>
--- a/CLT_ Timber_types.xlsx
+++ b/CLT_ Timber_types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SATNOORK\Documents\GitHub\CLT-LCA-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SATNOORK\Desktop\CLT Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757F9ADC-A211-4AB0-AF0F-771323BB3887}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E49FB8-0D42-4FD0-99A5-8DBED635DFAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4B413383-7D80-4A55-A275-D2B856FA8E62}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B413383-7D80-4A55-A275-D2B856FA8E62}"/>
   </bookViews>
   <sheets>
     <sheet name="ALSC PS 20 Lumber Species" sheetId="1" r:id="rId1"/>
@@ -1202,23 +1202,23 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -1236,7 +1236,7 @@
       </c>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>57</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>271</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>1.2471655328798188</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>222</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>1.2585034013605443</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>202</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>1.3125763125763126</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>181</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>1.2716450216450217</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>304</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>1.228878648233487</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>140</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>140</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>1.2471655328798188</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>58</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>607</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>1.3038548752834467</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>59</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>201223</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>1.2471655328798188</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>223</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>60</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>121</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>1.2626262626262625</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>263</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>1.2548262548262548</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>140</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>140</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>1.2566137566137567</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>267</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>1.2585034013605443</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>140</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>261</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>1.2548262548262548</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>61</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>104105</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>1.2531328320802007</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>270</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>1.2755102040816326</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>301</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>1.2755102040816326</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>62</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>183</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>321</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>1.2896825396825398</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>126</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>1.2876579203109815</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>64</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>363</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>29</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>261</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>223</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>223</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>1.287001287001287</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>101</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>1.2797619047619049</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>366</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>281</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>1.2844611528822054</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>140</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>167</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>1.3171225937183386</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>221</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>1.2531328320802007</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>364</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>224</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>1.2605042016806722</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>367</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>140</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>1.2925170068027212</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>140</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>141</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>1.3007054673721341</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>140</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>140</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>65</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>341</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>1.2531328320802007</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>140</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>125</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>1.3157894736842104</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>123</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>1.287001287001287</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>122</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>1.2987012987012987</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>269</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
         <v>265266</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>1.2626262626262625</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>305</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>1.287001287001287</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>384</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>66</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>140</v>
       </c>
@@ -3850,17 +3850,17 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="6" customWidth="1"/>
     <col min="2" max="2" width="24" style="6" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="25.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>70</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>101</v>
       </c>
@@ -3896,7 +3896,7 @@
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>104</v>
       </c>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>105</v>
       </c>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>121</v>
       </c>
@@ -3953,7 +3953,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>122</v>
       </c>
@@ -3972,7 +3972,7 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>123</v>
       </c>
@@ -3991,7 +3991,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>124</v>
       </c>
@@ -4010,7 +4010,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>125</v>
       </c>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>141</v>
       </c>
@@ -4048,7 +4048,7 @@
       </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>167</v>
       </c>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>181</v>
       </c>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>183</v>
       </c>
@@ -4105,7 +4105,7 @@
       </c>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>201</v>
       </c>
@@ -4124,7 +4124,7 @@
       </c>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>202</v>
       </c>
@@ -4143,7 +4143,7 @@
       </c>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>221</v>
       </c>
@@ -4162,7 +4162,7 @@
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>222</v>
       </c>
@@ -4181,7 +4181,7 @@
       </c>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:6" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>223</v>
       </c>
@@ -4200,7 +4200,7 @@
       </c>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>224</v>
       </c>
@@ -4219,7 +4219,7 @@
       </c>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>261</v>
       </c>
@@ -4238,7 +4238,7 @@
       </c>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>263</v>
       </c>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>265</v>
       </c>
@@ -4276,7 +4276,7 @@
       </c>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>266</v>
       </c>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>267</v>
       </c>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>269</v>
       </c>
@@ -4333,7 +4333,7 @@
       </c>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>270</v>
       </c>
@@ -4352,7 +4352,7 @@
       </c>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>271</v>
       </c>
@@ -4371,7 +4371,7 @@
       </c>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>281</v>
       </c>
@@ -4390,7 +4390,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>301</v>
       </c>
@@ -4409,7 +4409,7 @@
       </c>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>304</v>
       </c>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>305</v>
       </c>
@@ -4447,7 +4447,7 @@
       </c>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>321</v>
       </c>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>341</v>
       </c>
@@ -4485,7 +4485,7 @@
       </c>
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>361</v>
       </c>
@@ -4504,7 +4504,7 @@
       </c>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>363</v>
       </c>
@@ -4523,7 +4523,7 @@
       </c>
       <c r="F35" s="11"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>364</v>
       </c>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>366</v>
       </c>
@@ -4561,7 +4561,7 @@
       </c>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>367</v>
       </c>
@@ -4580,7 +4580,7 @@
       </c>
       <c r="F38" s="11"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>384</v>
       </c>
@@ -4599,7 +4599,7 @@
       </c>
       <c r="F39" s="11"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>126</v>
       </c>
@@ -4618,7 +4618,7 @@
       </c>
       <c r="F40" s="11"/>
     </row>
-    <row r="41" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>607</v>
       </c>

</xml_diff>